<commit_message>
messing with new dissolution vs growth
</commit_message>
<xml_diff>
--- a/raw/Long deliniated lengths.xlsx
+++ b/raw/Long deliniated lengths.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina.SCCWRP2K\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\crab_eval\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB57175C-C500-4AC3-ABFF-CF77D187548C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23550" windowHeight="11475" tabRatio="863"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23550" windowHeight="11475" tabRatio="863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="4" r:id="rId1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,12 +448,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E299" sqref="E299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6392,7 +6393,7 @@
         <v>8.94</v>
       </c>
       <c r="E296">
-        <v>966</v>
+        <v>9.66</v>
       </c>
       <c r="F296" s="1">
         <v>2</v>

</xml_diff>